<commit_message>
fixed set_invalid_row method and deleted some unused files
</commit_message>
<xml_diff>
--- a/spec/files/users_invalid.xlsx
+++ b/spec/files/users_invalid.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Username</t>
   </si>
@@ -184,11 +184,11 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A8" activeCellId="0" pane="topLeft" sqref="A8"/>
+      <selection activeCell="B8" activeCellId="0" pane="topLeft" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -279,7 +279,9 @@
       <c r="A7" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>5</v>
+      </c>
       <c r="C7" s="0" t="s">
         <v>6</v>
       </c>
@@ -322,8 +324,9 @@
     <hyperlink display="email1@test.com" ref="B4" r:id="rId3"/>
     <hyperlink display="email1@test.com" ref="B5" r:id="rId4"/>
     <hyperlink display="email1@test.com" ref="B6" r:id="rId5"/>
-    <hyperlink display="email1@test.com" ref="B8" r:id="rId6"/>
-    <hyperlink display="email1@test.com" ref="B9" r:id="rId7"/>
+    <hyperlink display="email1@test.com" ref="B7" r:id="rId6"/>
+    <hyperlink display="email1@test.com" ref="B8" r:id="rId7"/>
+    <hyperlink display="email1@test.com" ref="B9" r:id="rId8"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -347,7 +350,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -372,7 +375,7 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.7490196078431"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.8117647058824"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>